<commit_message>
update remaining Transboundary tables to 2023
</commit_message>
<xml_diff>
--- a/data-raw/TBR/TBR data_updated2023.xlsx
+++ b/data-raw/TBR/TBR data_updated2023.xlsx
@@ -5,32 +5,32 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/alaska-salmon-reports/TBR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/Alaskan-catch-of-BC-salmon/data-raw/TBR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC945FF1-0788-DE42-9547-62A43C053048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C846FD2-8CA6-254B-A870-6E380A8D9C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="500" windowWidth="24700" windowHeight="16140" activeTab="6" xr2:uid="{4242C904-F905-416D-8DC3-5684C10FD238}"/>
+    <workbookView xWindow="1900" yWindow="2800" windowWidth="24700" windowHeight="16140" firstSheet="13" activeTab="14" xr2:uid="{4242C904-F905-416D-8DC3-5684C10FD238}"/>
   </bookViews>
   <sheets>
-    <sheet name="stikine CN RR" sheetId="1" r:id="rId1"/>
-    <sheet name="stikine CN D108 catch" sheetId="2" r:id="rId2"/>
-    <sheet name="stikine CN D108 prop" sheetId="3" r:id="rId3"/>
-    <sheet name="B1 106 harvest" sheetId="4" r:id="rId4"/>
-    <sheet name="B2 108 harvest" sheetId="5" r:id="rId5"/>
-    <sheet name="B21 Stikine SX" sheetId="19" r:id="rId6"/>
+    <sheet name="TBR.stikine.chinook.rr" sheetId="1" r:id="rId1"/>
+    <sheet name="TBR.stikine.cn.d108.catch" sheetId="2" r:id="rId2"/>
+    <sheet name="TBR.stikine.cn.d108.prop" sheetId="3" r:id="rId3"/>
+    <sheet name="TBR.106.harvest" sheetId="4" r:id="rId4"/>
+    <sheet name="TBR.108.harvest" sheetId="5" r:id="rId5"/>
+    <sheet name="TBR.stikine.river" sheetId="19" r:id="rId6"/>
     <sheet name="D108 D111 CN GSI 15 16 17" sheetId="7" r:id="rId7"/>
-    <sheet name="D5 Taku CN RR" sheetId="9" r:id="rId8"/>
-    <sheet name="G1 G2 G4 CN GSI D108 D111" sheetId="8" r:id="rId9"/>
-    <sheet name="D1 111 harvest" sheetId="6" r:id="rId10"/>
-    <sheet name="D20 Taku CO" sheetId="10" r:id="rId11"/>
-    <sheet name="D19 D111 CO Catch" sheetId="11" r:id="rId12"/>
-    <sheet name="D7 D111 SX catch" sheetId="13" r:id="rId13"/>
-    <sheet name="D15 TAKU SX RR" sheetId="14" r:id="rId14"/>
-    <sheet name="D9 D111 SX TAKU GSI" sheetId="12" r:id="rId15"/>
-    <sheet name="E4 ALSEK CN" sheetId="15" r:id="rId16"/>
-    <sheet name="E9 ALSEK SX" sheetId="16" r:id="rId17"/>
-    <sheet name="ALSEK CO PK CM catch" sheetId="18" r:id="rId18"/>
+    <sheet name="TBR.D5.Taku.Lchinook" sheetId="9" r:id="rId8"/>
+    <sheet name="TBR.chinook.GSI.D108.D111" sheetId="8" r:id="rId9"/>
+    <sheet name="TBR.D111harvest" sheetId="6" r:id="rId10"/>
+    <sheet name="TBR.D20.Taku.CO" sheetId="10" r:id="rId11"/>
+    <sheet name="TBR.D111.co.catch" sheetId="11" r:id="rId12"/>
+    <sheet name="TBR.D111.sx.catch" sheetId="13" r:id="rId13"/>
+    <sheet name="TBR.D15.Taku.SX" sheetId="14" r:id="rId14"/>
+    <sheet name="TBR.D111.sx.taku.GSI" sheetId="12" r:id="rId15"/>
+    <sheet name="TBR.ALSEK.chinook" sheetId="15" r:id="rId16"/>
+    <sheet name="TBR.ALSEK.sockeye" sheetId="16" r:id="rId17"/>
+    <sheet name="TBR.ALSEK.co.pk.cm.catch" sheetId="18" r:id="rId18"/>
     <sheet name="E14 ALSEK SEAK CO PK CM" sheetId="17" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -304,7 +304,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,12 +314,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -344,7 +338,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,7 +655,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1273,7 +1266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAE45292-89B8-C34C-9811-775368BB53A5}">
   <dimension ref="A1:P88"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
@@ -3001,7 +2994,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4687,7 +4680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC66C08-F54E-48E6-907D-D6FB95DCE877}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
@@ -5665,7 +5658,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5681,1157 +5674,1155 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+      <c r="A2" s="6">
         <v>1984</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>88272</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>70894</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>105650</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>27292</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>60980</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>57619</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <v>145891</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="6">
         <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>1985</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>84479</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>67333</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>101625</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>14411</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>70068</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>74287</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
         <v>158766</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>1986</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6">
         <v>14939</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6">
         <v>60644</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>1987</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>56362</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>45590</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>67134</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>13887</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>42475</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>54963</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <v>111325</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="6">
         <v>0.62</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>1988</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>55580</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>44648</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>66512</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>12967</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>42613</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>25785</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>81365</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>0.48</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>1989</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>80997</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>65787</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>96207</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>18805</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>62192</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>63366</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>144363</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>1990</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>75801</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>61839</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>89763</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>21474</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>54327</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>109285</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>185086</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>0.71</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>1991</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>104895</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>85097</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>124693</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>25380</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>79515</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>105271</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <v>210166</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <v>0.62</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>1992</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>99643</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>81401</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>117885</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>29862</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>69781</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>121176</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <v>220819</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <v>0.68</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>1993</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>92933</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>76231</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>109635</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>33523</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>59410</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>142089</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>235022</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>1994</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>90128</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>73666</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>106590</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>29001</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>61127</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <v>98063</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <v>188191</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="6">
         <v>0.68</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>1995</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>104242</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>85180</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>123304</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>32711</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>71531</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <v>91984</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <v>196226</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="6">
         <v>0.64</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>1996</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>97477</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>79901</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>115053</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>42025</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>55452</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="6">
         <v>187727</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="6">
         <v>285204</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="6">
         <v>0.81</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>1997</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>73255</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>59861</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>86649</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>24352</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>48903</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <v>79127</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="6">
         <v>152382</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="6">
         <v>0.68</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
+      <c r="A16" s="6">
         <v>1998</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>64755</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>52617</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>76893</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>19277</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>45478</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <v>49832</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="6">
         <v>114587</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="6">
         <v>0.6</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <v>1999</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>83588</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>67816</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>99360</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>21151</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>62437</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <v>63058</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="6">
         <v>146646</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="6">
         <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
+      <c r="A18" s="6">
         <v>2000</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>83190</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>68024</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="6">
         <v>98356</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>28468</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <v>54722</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <v>131262</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="6">
         <v>214452</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="6">
         <v>0.74</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="7">
+      <c r="A19" s="6">
         <v>2001</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>132502</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>108404</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>156600</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>48117</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>84385</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>204433</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="6">
         <v>336935</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="6">
         <v>0.75</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
+      <c r="A20" s="6">
         <v>2002</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>94605</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>77331</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <v>111879</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>31726</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>62879</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="6">
         <v>116400</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="6">
         <v>211005</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="6">
         <v>0.7</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="7">
+      <c r="A21" s="6">
         <v>2003</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>133593</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>108917</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>158269</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>33024</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>100569</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="6">
         <v>136942</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="6">
         <v>270535</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="6">
         <v>0.63</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="7">
+      <c r="A22" s="6">
         <v>2004</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <v>85257</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>69601</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
         <v>100913</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>20359</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="6">
         <v>64898</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="6">
         <v>77012</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="6">
         <v>162269</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="6">
         <v>0.6</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="7">
+      <c r="A23" s="6">
         <v>2005</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <v>87496</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <v>70454</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>104538</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>22102</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <v>65394</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="6">
         <v>46089</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="6">
         <v>133585</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="6">
         <v>0.51</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
+      <c r="A24" s="6">
         <v>2006</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <v>106545</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>86195</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
         <v>126895</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>21446</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <v>85099</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="6">
         <v>65828</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="6">
         <v>172373</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="6">
         <v>0.51</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="7">
+      <c r="A25" s="6">
         <v>2007</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <v>60320</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <v>49616</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="6">
         <v>71024</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
         <v>17249</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <v>43071</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="6">
         <v>65129</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="6">
         <v>125449</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="6">
         <v>0.66</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="7">
+      <c r="A26" s="6">
         <v>2008</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <v>78031</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>62737</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="6">
         <v>93325</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <v>19509</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="6">
         <v>58522</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="6">
         <v>75692</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="6">
         <v>153723</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="6">
         <v>0.62</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="7">
+      <c r="A27" s="6">
         <v>2009</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="6">
         <v>59817</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <v>47343</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>72291</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <v>11260</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="6">
         <v>48557</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="6">
         <v>36232</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="6">
         <v>96049</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="6">
         <v>0.49</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="7">
+      <c r="A28" s="6">
         <v>2010</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="6">
         <v>80747</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
         <v>64679</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="6">
         <v>96815</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="6">
         <v>20661</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="6">
         <v>60086</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="6">
         <v>46767</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="6">
         <v>127514</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="6">
         <v>0.53</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="7">
+      <c r="A29" s="6">
         <v>2011</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="6">
         <v>82116</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <v>66634</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="6">
         <v>97598</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="6">
         <v>24543</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="6">
         <v>57573</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="6">
         <v>71805</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="6">
         <v>153921</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="6">
         <v>0.63</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="7">
+      <c r="A30" s="6">
         <v>2012</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="6">
         <v>102670</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <v>83602</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="6">
         <v>121738</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="6">
         <v>30113</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="6">
         <v>72557</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="6">
         <v>50736</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H30" s="6">
         <v>153406</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="6">
         <v>0.53</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="7">
+      <c r="A31" s="6">
         <v>2013</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="6">
         <v>88535</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <v>71523</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>105547</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="6">
         <v>25173</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="6">
         <v>63362</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="6">
         <v>100144</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="6">
         <v>188679</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31" s="6">
         <v>0.66</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="7">
+      <c r="A32" s="6">
         <v>2014</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="6">
         <v>68532</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="6">
         <v>55818</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="6">
         <v>81246</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="6">
         <v>17795</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="6">
         <v>50737</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="6">
         <v>33226</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="6">
         <v>101758</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="6">
         <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="7">
+      <c r="A33" s="6">
         <v>2015</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="6">
         <v>102506</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="6">
         <v>81982</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="6">
         <v>123030</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="6">
         <v>19849</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="6">
         <v>82657</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="6">
         <v>42054</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33" s="6">
         <v>144560</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33" s="6">
         <v>0.43</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="7">
+      <c r="A34" s="6">
         <v>2016</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="6">
         <v>146294</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="6">
         <v>119726</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="6">
         <v>172862</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="6">
         <v>37434</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="6">
         <v>108860</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="6">
         <v>74874</v>
       </c>
-      <c r="H34" s="7">
+      <c r="H34" s="6">
         <v>221168</v>
       </c>
-      <c r="I34" s="7">
+      <c r="I34" s="6">
         <v>0.51</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="7">
+      <c r="A35" s="6">
         <v>2017</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="6">
         <v>91164</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="6">
         <v>81104</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="6">
         <v>101224</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="6">
         <v>30379</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="6">
         <v>60785</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="6">
         <v>74604</v>
       </c>
-      <c r="H35" s="7">
+      <c r="H35" s="6">
         <v>165768</v>
       </c>
-      <c r="I35" s="7">
+      <c r="I35" s="6">
         <v>0.63</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="7">
+      <c r="A36" s="6">
         <v>2018</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="6">
         <v>84806</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="6">
         <v>74394</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="6">
         <v>95218</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="6">
         <v>17962</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="6">
         <v>66844</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="6">
         <v>27514</v>
       </c>
-      <c r="H36" s="7">
+      <c r="H36" s="6">
         <v>112320</v>
       </c>
-      <c r="I36" s="7">
+      <c r="I36" s="6">
         <v>0.4</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="7">
+      <c r="A37" s="6">
         <v>2019</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="6">
         <v>103152</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="6">
         <v>94587</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="6">
         <v>111717</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="6">
         <v>21481</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="6">
         <v>81671</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="6">
         <v>68226</v>
       </c>
-      <c r="H37" s="7">
+      <c r="H37" s="6">
         <v>171378</v>
       </c>
-      <c r="I37" s="7">
+      <c r="I37" s="6">
         <v>0.54</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="7">
+      <c r="A38" s="6">
         <v>2020</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="6">
         <v>112677</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="6">
         <v>92650</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="6">
         <v>132704</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="6">
         <v>11780</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="6">
         <v>100897</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G38" s="6">
         <v>9472</v>
       </c>
-      <c r="H38" s="7">
+      <c r="H38" s="6">
         <v>122149</v>
       </c>
-      <c r="I38" s="7">
+      <c r="I38" s="6">
         <v>0.19</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="7">
+      <c r="A39" s="6">
         <v>2021</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="6">
         <v>182115</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="6">
         <v>138892</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="6">
         <v>225338</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="6">
         <v>18485</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="6">
         <v>163630</v>
       </c>
-      <c r="G39" s="7">
+      <c r="G39" s="6">
         <v>38784</v>
       </c>
-      <c r="H39" s="7">
+      <c r="H39" s="6">
         <v>220899</v>
       </c>
-      <c r="I39" s="7">
+      <c r="I39" s="6">
         <v>0.27</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="7">
+      <c r="A40" s="6">
         <v>2022</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="6">
         <v>121046</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="6">
         <v>103395</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="6">
         <v>138697</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="6">
         <v>27605</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="6">
         <v>93441</v>
       </c>
-      <c r="G40" s="7">
+      <c r="G40" s="6">
         <v>90458</v>
       </c>
-      <c r="H40" s="7">
+      <c r="H40" s="6">
         <v>211504</v>
       </c>
-      <c r="I40" s="7">
+      <c r="I40" s="6">
         <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="6">
-        <v>2023</v>
-      </c>
+      <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -6850,7 +6841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DAAC1C-3D33-43C1-9C0F-E926AA8F992C}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -8291,7 +8282,7 @@
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C68" sqref="C68"/>
@@ -16344,9 +16335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{152C36A6-EF70-4883-B9E3-7E0A8DA2ED57}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17286,7 +17275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6975576C-EC9F-45D0-920C-79EEAB503992}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -17853,7 +17842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C11D9CE-B7CC-4FB1-9F9A-6BF4E3ACD765}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
@@ -18774,7 +18763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC9E15F-45E5-4657-A0F4-93AE7540D79D}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>

</xml_diff>